<commit_message>
* needed to remove min, max from prob in decision tree so can deterministic sensitivity analysis assign_branch_val
* use mapply in main model loop so can change cohort size for each scenario

* make ce plane plots
</commit_message>
<xml_diff>
--- a/data/scenario_parameters_predicted.xlsx
+++ b/data/scenario_parameters_predicted.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngreen1\Google Drive\ACE -- LTBI screening in hospital\R code\LTBIhospitalScreenACE\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Google Drive\ACE -- LTBI screening in hospital\R code\LTBIhospitalScreenACE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="p" sheetId="1" r:id="rId1"/>
-    <sheet name="cost" sheetId="2" r:id="rId2"/>
+    <sheet name="cost" sheetId="2" r:id="rId1"/>
+    <sheet name="p" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t>Agree to Screen</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="10">
   <si>
     <t>scenario</t>
   </si>
@@ -403,11 +400,318 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>144</v>
+      </c>
+      <c r="C2">
+        <v>144</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>144</v>
+      </c>
+      <c r="C3">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>144</v>
+      </c>
+      <c r="C4">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>144</v>
+      </c>
+      <c r="C5">
+        <v>144</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>147</v>
+      </c>
+      <c r="C6">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>147</v>
+      </c>
+      <c r="C7">
+        <v>147</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>147</v>
+      </c>
+      <c r="C8">
+        <v>147</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>147</v>
+      </c>
+      <c r="C9">
+        <v>147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>144</v>
+      </c>
+      <c r="C10">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>144</v>
+      </c>
+      <c r="C11">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>144</v>
+      </c>
+      <c r="C12">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>144</v>
+      </c>
+      <c r="C13">
+        <v>144</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>147</v>
+      </c>
+      <c r="C14">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>147</v>
+      </c>
+      <c r="C15">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>147</v>
+      </c>
+      <c r="C16">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>147</v>
+      </c>
+      <c r="C17">
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,19 +725,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -457,90 +761,59 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.92631580000000002</v>
+        <v>0.97297299999999998</v>
       </c>
       <c r="B3">
-        <v>0.94965029999999995</v>
+        <v>0.93522269999999996</v>
       </c>
       <c r="C3">
         <f>1-A3</f>
-        <v>7.3684199999999977E-2</v>
+        <v>2.7027000000000023E-2</v>
       </c>
       <c r="D3">
         <f>1-B3</f>
-        <v>5.0349700000000053E-2</v>
+        <v>6.4777300000000038E-2</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.92631580000000002</v>
+      </c>
+      <c r="B4">
+        <v>0.94965029999999995</v>
+      </c>
+      <c r="C4">
+        <f>1-A4</f>
+        <v>7.3684199999999977E-2</v>
+      </c>
+      <c r="D4">
+        <f>1-B4</f>
+        <v>5.0349700000000053E-2</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.92631580000000002</v>
+      </c>
+      <c r="B5">
+        <v>0.94965029999999995</v>
+      </c>
+      <c r="C5">
+        <f>1-A5</f>
+        <v>7.3684199999999977E-2</v>
+      </c>
+      <c r="D5">
+        <f>1-B5</f>
+        <v>5.0349700000000053E-2</v>
+      </c>
+      <c r="E5">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>